<commit_message>
update report of operators
</commit_message>
<xml_diff>
--- a/uk.ac.york.cs.emu.eol.lives.mutations.executor/csv_files/all_operators.xlsx
+++ b/uk.ac.york.cs.emu.eol.lives.mutations.executor/csv_files/all_operators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AFADF_F/Git/Fhma/MT_EOL/uk.ac.york.cs.emu.eol.lives.mutations.executor/csv_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CFF8B1-1BE2-4842-AA8A-EE1ED327BAAD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE13512-8612-0844-AC56-E756C90D685C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="440" windowWidth="28040" windowHeight="17060" xr2:uid="{F273EC95-D1FA-5641-97F6-083E7E98DC84}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Mutation Operator</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>CMO-S-DEL(PropertyCallExpression target)</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -554,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E327F6-4762-7445-A383-F8909480EFBD}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2222,6 +2225,57 @@
         <v>100</v>
       </c>
     </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="3">
+        <f>SUM(B2:B42)</f>
+        <v>5436</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" ref="C43:G43" si="5">SUM(C2:C42)</f>
+        <v>2294</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="5"/>
+        <v>787</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="5"/>
+        <v>1131</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="5"/>
+        <v>502</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" si="5"/>
+        <v>722</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C44" s="3">
+        <f>C43/B43*100</f>
+        <v>42.200147167034586</v>
+      </c>
+      <c r="D44" s="3">
+        <f>D43/B43*100</f>
+        <v>14.477557027225901</v>
+      </c>
+      <c r="E44" s="3">
+        <f>E43/B43*100</f>
+        <v>20.805739514348787</v>
+      </c>
+      <c r="F44" s="3">
+        <f>F43/B43*100</f>
+        <v>9.234731420161884</v>
+      </c>
+      <c r="G44" s="3">
+        <f>G43/B43*100</f>
+        <v>13.281824871228846</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:L42">
     <sortCondition descending="1" ref="J2:J42"/>

</xml_diff>

<commit_message>
add some changes to csv_files update mutation lives
</commit_message>
<xml_diff>
--- a/uk.ac.york.cs.emu.eol.lives.mutations.executor/csv_files/all_operators.xlsx
+++ b/uk.ac.york.cs.emu.eol.lives.mutations.executor/csv_files/all_operators.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AFADF_F/Git/Fhma/MT_EOL/uk.ac.york.cs.emu.eol.lives.mutations.executor/csv_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE13512-8612-0844-AC56-E756C90D685C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78C7CBE-02FE-2B4C-9FD9-0EA5D743762D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="440" windowWidth="28040" windowHeight="17060" xr2:uid="{F273EC95-D1FA-5641-97F6-083E7E98DC84}"/>
+    <workbookView xWindow="380" yWindow="440" windowWidth="28040" windowHeight="17060" activeTab="1" xr2:uid="{F273EC95-D1FA-5641-97F6-083E7E98DC84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>Mutation Operator</t>
   </si>
@@ -559,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E327F6-4762-7445-A383-F8909480EFBD}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2286,4 +2292,791 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797ABAB8-AC0E-B14F-90A2-EF1D146FF9AA}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <f>C2+D2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E31" si="0">C3+D3</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="F4" s="2">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
+        <v>145</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="F5" s="2">
+        <v>62</v>
+      </c>
+      <c r="G5" s="2">
+        <v>17</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F6" s="2">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2">
+        <v>85</v>
+      </c>
+      <c r="C7" s="2">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2">
+        <v>39</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="F7" s="2">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45</v>
+      </c>
+      <c r="C8" s="2">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F8" s="2">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2">
+        <v>209</v>
+      </c>
+      <c r="C9" s="2">
+        <v>56</v>
+      </c>
+      <c r="D9" s="2">
+        <v>36</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="F9" s="2">
+        <v>68</v>
+      </c>
+      <c r="G9" s="2">
+        <v>32</v>
+      </c>
+      <c r="H9" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2">
+        <v>160</v>
+      </c>
+      <c r="C10" s="2">
+        <v>72</v>
+      </c>
+      <c r="D10" s="2">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="F10" s="2">
+        <v>51</v>
+      </c>
+      <c r="G10" s="2">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2">
+        <v>102</v>
+      </c>
+      <c r="C11" s="2">
+        <v>64</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="F11" s="2">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2">
+        <v>170</v>
+      </c>
+      <c r="C12" s="2">
+        <v>99</v>
+      </c>
+      <c r="D12" s="2">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="F12" s="2">
+        <v>50</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F13" s="2">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>825</v>
+      </c>
+      <c r="C14" s="2">
+        <v>335</v>
+      </c>
+      <c r="D14" s="2">
+        <v>161</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>496</v>
+      </c>
+      <c r="F14" s="2">
+        <v>234</v>
+      </c>
+      <c r="G14" s="2">
+        <v>95</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2">
+        <v>96</v>
+      </c>
+      <c r="C15" s="2">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F15" s="2">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2">
+        <v>10</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2">
+        <v>230</v>
+      </c>
+      <c r="C16" s="2">
+        <v>109</v>
+      </c>
+      <c r="D16" s="2">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="F16" s="2">
+        <v>62</v>
+      </c>
+      <c r="G16" s="2">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2">
+        <v>119</v>
+      </c>
+      <c r="C17" s="2">
+        <v>60</v>
+      </c>
+      <c r="D17" s="2">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F17" s="2">
+        <v>28</v>
+      </c>
+      <c r="G17" s="2">
+        <v>16</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2">
+        <v>529</v>
+      </c>
+      <c r="C18" s="2">
+        <v>297</v>
+      </c>
+      <c r="D18" s="2">
+        <v>84</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>381</v>
+      </c>
+      <c r="F18" s="2">
+        <v>123</v>
+      </c>
+      <c r="G18" s="2">
+        <v>25</v>
+      </c>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2">
+        <v>581</v>
+      </c>
+      <c r="C19" s="2">
+        <v>324</v>
+      </c>
+      <c r="D19" s="2">
+        <v>99</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>423</v>
+      </c>
+      <c r="F19" s="2">
+        <v>125</v>
+      </c>
+      <c r="G19" s="2">
+        <v>33</v>
+      </c>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2">
+        <v>178</v>
+      </c>
+      <c r="C20" s="2">
+        <v>108</v>
+      </c>
+      <c r="D20" s="2">
+        <v>32</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="F20" s="2">
+        <v>30</v>
+      </c>
+      <c r="G20" s="2">
+        <v>8</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2">
+        <v>205</v>
+      </c>
+      <c r="C21" s="2">
+        <v>69</v>
+      </c>
+      <c r="D21" s="2">
+        <v>24</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="F21" s="2">
+        <v>32</v>
+      </c>
+      <c r="G21" s="2">
+        <v>16</v>
+      </c>
+      <c r="H21" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4</v>
+      </c>
+      <c r="G22" s="2">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2">
+        <v>160</v>
+      </c>
+      <c r="C23" s="2">
+        <v>101</v>
+      </c>
+      <c r="D23" s="2">
+        <v>25</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="F23" s="2">
+        <v>22</v>
+      </c>
+      <c r="G23" s="2">
+        <v>12</v>
+      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="2">
+        <v>205</v>
+      </c>
+      <c r="C24" s="2">
+        <v>33</v>
+      </c>
+      <c r="D24" s="2">
+        <v>21</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="F24" s="2">
+        <v>28</v>
+      </c>
+      <c r="G24" s="2">
+        <v>58</v>
+      </c>
+      <c r="H24" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="2">
+        <v>97</v>
+      </c>
+      <c r="C25" s="2">
+        <v>36</v>
+      </c>
+      <c r="D25" s="2">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="F25" s="2">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2">
+        <v>18</v>
+      </c>
+      <c r="H25" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="2">
+        <v>103</v>
+      </c>
+      <c r="C26" s="2">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="F26" s="2">
+        <v>11</v>
+      </c>
+      <c r="G26" s="2">
+        <v>16</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="2">
+        <v>103</v>
+      </c>
+      <c r="C27" s="2">
+        <v>70</v>
+      </c>
+      <c r="D27" s="2">
+        <v>6</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="F27" s="2">
+        <v>10</v>
+      </c>
+      <c r="G27" s="2">
+        <v>17</v>
+      </c>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="2">
+        <v>212</v>
+      </c>
+      <c r="C28" s="2">
+        <v>135</v>
+      </c>
+      <c r="D28" s="2">
+        <v>34</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="0"/>
+        <v>169</v>
+      </c>
+      <c r="F28" s="2">
+        <v>19</v>
+      </c>
+      <c r="G28" s="2">
+        <v>24</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="2">
+        <v>49</v>
+      </c>
+      <c r="C29" s="2">
+        <v>34</v>
+      </c>
+      <c r="D29" s="2">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="F29" s="2">
+        <v>3</v>
+      </c>
+      <c r="G29" s="2">
+        <v>4</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="2">
+        <v>17</v>
+      </c>
+      <c r="C30" s="2">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2">
+        <v>12</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="2">
+        <v>71</v>
+      </c>
+      <c r="C31" s="2">
+        <v>62</v>
+      </c>
+      <c r="D31" s="2">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2">
+        <v>5</v>
+      </c>
+      <c r="H31" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>